<commit_message>
Add Account Detail (#189)
* Add scrolling

* Add mobile nav

* Add account page

* Add transaction

* WIP

* Add create transaction

* Add banking forms

* Fix

* Add bank and investment transactions

* Update todo

* Add clean up

* Update todo

* Add disabeld

* Add

* Add delete

* Edit

* Update

* Add edit

* Update todo

* Update todo

* Fix code style
</commit_message>
<xml_diff>
--- a/references/Tables.xlsx
+++ b/references/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AMAABCA\eric-bach\pecuniary\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pecuniary\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE7AC92-9ADF-47E9-878F-9FDF72728DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B6823B-8023-4E0E-AEAF-6CAC5A1712F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20865" yWindow="4020" windowWidth="25380" windowHeight="15270" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
+    <workbookView xWindow="3735" yWindow="2505" windowWidth="33750" windowHeight="18555" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable v2" sheetId="9" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="187">
   <si>
     <t>name</t>
   </si>
@@ -643,6 +632,45 @@
   </si>
   <si>
     <t>Get an aggregate</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sk </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Sort Key)</t>
+    </r>
+  </si>
+  <si>
+    <t>investment-transaction</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>banking</t>
+  </si>
+  <si>
+    <t>investment</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>invesment-transaction</t>
+  </si>
+  <si>
+    <t>&lt;transId&gt;</t>
+  </si>
+  <si>
+    <t>&lt;posId&gt;</t>
   </si>
 </sst>
 </file>
@@ -858,6 +886,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -884,9 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1203,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C67D2A-5435-4CFA-A6DE-EEB96100D814}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,82 +1242,84 @@
     <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="4"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="9.140625" style="6"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="4"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="9.140625" style="6"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="9"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
-    </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>113</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="9"/>
+        <v>178</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -1305,28 +1335,31 @@
         <v>25</v>
       </c>
       <c r="G3" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="13"/>
+      <c r="M3" s="11"/>
       <c r="N3" s="13"/>
-      <c r="O3" s="2"/>
+      <c r="O3" s="13"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="3"/>
+      <c r="Q3" s="2"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="12" t="s">
         <v>122</v>
       </c>
@@ -1339,30 +1372,33 @@
       <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="15"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="1"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="1"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-      <c r="U4" s="6"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="T4" s="4"/>
+      <c r="V4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1378,27 +1414,30 @@
         <v>25</v>
       </c>
       <c r="G5" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="I5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="15"/>
+      <c r="M5" s="12"/>
       <c r="N5" s="15"/>
-      <c r="O5" s="1"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="1"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-      <c r="U5" s="6"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="T5" s="4"/>
+      <c r="V5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="12" t="s">
         <v>122</v>
       </c>
@@ -1411,30 +1450,33 @@
       <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
-      <c r="M6" s="15"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="15"/>
-      <c r="O6" s="1"/>
+      <c r="O6" s="15"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="4"/>
+      <c r="Q6" s="1"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
-      <c r="U6" s="6"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="T6" s="4"/>
+      <c r="V6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -1450,27 +1492,30 @@
         <v>25</v>
       </c>
       <c r="G7" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-      <c r="M7" s="15"/>
+      <c r="M7" s="12"/>
       <c r="N7" s="15"/>
-      <c r="O7" s="1"/>
+      <c r="O7" s="15"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="4"/>
+      <c r="Q7" s="1"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
-      <c r="U7" s="6"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
+      <c r="T7" s="4"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="12" t="s">
         <v>122</v>
       </c>
@@ -1483,30 +1528,33 @@
       <c r="F8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="15"/>
+      <c r="M8" s="12"/>
       <c r="N8" s="15"/>
-      <c r="O8" s="1"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="4"/>
+      <c r="Q8" s="1"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="U8" s="8"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="T8" s="4"/>
+      <c r="V8" s="8"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="18" t="s">
@@ -1519,82 +1567,88 @@
         <v>159</v>
       </c>
       <c r="F9" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="H9" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="J9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="L9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="M9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="15"/>
       <c r="N9" s="15"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="1"/>
       <c r="S9" s="4"/>
-      <c r="U9" s="8"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="W9" s="8"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="12" t="s">
         <v>122</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>26</v>
+        <v>184</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="16">
+      <c r="H10" s="16">
         <v>44662</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="12">
+      <c r="J10" s="12">
         <v>100</v>
       </c>
-      <c r="J10" s="15">
+      <c r="K10" s="15">
         <v>125.43</v>
       </c>
-      <c r="K10" s="15">
+      <c r="L10" s="15">
         <v>5.99</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="M10" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="M10" s="15"/>
       <c r="N10" s="15"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="1"/>
       <c r="S10" s="4"/>
-      <c r="U10" s="6"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -1607,82 +1661,88 @@
         <v>159</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="H11" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="I11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="J11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="K11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="L11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="M11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="15"/>
       <c r="N11" s="15"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="1"/>
       <c r="S11" s="4"/>
-      <c r="U11" s="6"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="12" t="s">
         <v>122</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>26</v>
+        <v>184</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="16">
+      <c r="H12" s="16">
         <v>44663</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="12">
+      <c r="J12" s="12">
         <v>50</v>
       </c>
-      <c r="J12" s="15">
+      <c r="K12" s="15">
         <v>138.19999999999999</v>
       </c>
-      <c r="K12" s="15">
+      <c r="L12" s="15">
         <v>4.95</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="15"/>
       <c r="N12" s="15"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="1"/>
       <c r="S12" s="4"/>
-      <c r="U12" s="6"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -1695,82 +1755,88 @@
         <v>159</v>
       </c>
       <c r="F13" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="H13" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="I13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="J13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="K13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="L13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="M13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="15"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="1"/>
       <c r="S13" s="4"/>
-      <c r="U13" s="6"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="12" t="s">
         <v>122</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="16">
+      <c r="H14" s="16">
         <v>44664</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="I14" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="12">
+      <c r="J14" s="12">
         <v>100</v>
       </c>
-      <c r="J14" s="15">
+      <c r="K14" s="15">
         <v>105.87</v>
       </c>
-      <c r="K14" s="15">
+      <c r="L14" s="15">
         <v>4.95</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="M14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="15"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="1"/>
       <c r="S14" s="4"/>
-      <c r="U14" s="6"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -1783,36 +1849,39 @@
         <v>159</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="J15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="18" t="s">
+      <c r="K15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="L15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="12"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="1"/>
       <c r="S15" s="4"/>
-      <c r="U15" s="6"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="12" t="s">
         <v>122</v>
       </c>
@@ -1822,39 +1891,42 @@
       <c r="E16" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="16">
+      <c r="F16" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="I16" s="16">
         <v>44664</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="J16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="12">
+      <c r="K16" s="12">
         <v>100</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="L16" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="1"/>
       <c r="S16" s="4"/>
-      <c r="U16" s="8"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="W16" s="8"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="18" t="s">
@@ -1867,42 +1939,45 @@
         <v>159</v>
       </c>
       <c r="F17" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="K17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="L17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="M17" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="20" t="s">
+      <c r="N17" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="O17" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="18" t="s">
+      <c r="P17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="Q17" s="1"/>
       <c r="S17" s="4"/>
-      <c r="U17" s="8"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="36"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="W17" s="8"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12" t="s">
         <v>122</v>
       </c>
@@ -1912,46 +1987,49 @@
       <c r="E18" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="H18" s="14"/>
+      <c r="I18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="12">
+      <c r="J18" s="12">
         <v>150</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="K18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="L18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="15">
+      <c r="M18" s="15">
         <f>12543+5.99+50*145.23+5.99</f>
         <v>19816.48</v>
       </c>
-      <c r="L18" s="15">
+      <c r="N18" s="15">
         <v>13458.52</v>
       </c>
-      <c r="M18" s="15">
+      <c r="O18" s="15">
         <v>18617.25</v>
       </c>
-      <c r="N18" s="12" t="s">
+      <c r="P18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="Q18" s="1"/>
       <c r="S18" s="4"/>
-      <c r="U18" s="6"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -1964,42 +2042,45 @@
         <v>159</v>
       </c>
       <c r="F19" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="H19" s="18"/>
+      <c r="I19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="J19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="K19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="L19" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="M19" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="20" t="s">
+      <c r="N19" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="20" t="s">
+      <c r="O19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="18" t="s">
+      <c r="P19" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="Q19" s="1"/>
       <c r="S19" s="4"/>
-      <c r="U19" s="6"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="36"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="12" t="s">
         <v>122</v>
       </c>
@@ -2009,43 +2090,46 @@
       <c r="E20" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="H20" s="14"/>
+      <c r="I20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="12">
+      <c r="J20" s="12">
         <v>100</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="K20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="L20" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="15">
+      <c r="M20" s="15">
         <f>50*867.23+5.99</f>
         <v>43367.49</v>
       </c>
-      <c r="L20" s="15">
+      <c r="N20" s="15">
         <v>60215.67</v>
       </c>
-      <c r="M20" s="15">
+      <c r="O20" s="15">
         <v>43367.49</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="P20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="U20" s="6"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>114</v>
       </c>
@@ -2079,8 +2163,9 @@
       <c r="K22" s="28" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="28"/>
+    </row>
+    <row r="23" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>174</v>
       </c>
@@ -2106,8 +2191,9 @@
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
-    </row>
-    <row r="24" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L23" s="29"/>
+    </row>
+    <row r="24" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>175</v>
       </c>
@@ -2127,8 +2213,9 @@
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
-    </row>
-    <row r="25" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="29"/>
+    </row>
+    <row r="25" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>152</v>
       </c>
@@ -2148,8 +2235,9 @@
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
-    </row>
-    <row r="26" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>170</v>
       </c>
@@ -2169,8 +2257,9 @@
       <c r="I26" s="29"/>
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
-    </row>
-    <row r="27" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="29"/>
+    </row>
+    <row r="27" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>123</v>
       </c>
@@ -2196,8 +2285,9 @@
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
-    </row>
-    <row r="28" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="29"/>
+    </row>
+    <row r="28" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>107</v>
       </c>
@@ -2219,8 +2309,9 @@
       <c r="I28" s="29"/>
       <c r="J28" s="29"/>
       <c r="K28" s="29"/>
-    </row>
-    <row r="29" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="29"/>
+    </row>
+    <row r="29" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>155</v>
       </c>
@@ -2234,7 +2325,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>140</v>
       </c>
@@ -2257,7 +2348,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>148</v>
       </c>
@@ -2280,26 +2371,26 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+    <row r="32" spans="1:23" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="E32" s="39" t="s">
+      <c r="E32" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="30" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2358,28 +2449,28 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="39" t="s">
+      <c r="D36" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="E36" s="39" t="s">
+      <c r="E36" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="F36" s="39" t="s">
+      <c r="F36" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="G36" s="39" t="s">
+      <c r="G36" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="30" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2414,7 +2505,7 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C1:N2"/>
+    <mergeCell ref="C1:O2"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A13:A14"/>
@@ -2465,23 +2556,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
       <c r="N1" s="10"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
@@ -2498,17 +2589,17 @@
       <c r="B2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
@@ -2518,10 +2609,10 @@
       <c r="T2" s="9"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -2554,8 +2645,8 @@
       <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
@@ -2584,10 +2675,10 @@
       <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -2618,8 +2709,8 @@
       <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
@@ -2648,10 +2739,10 @@
       <c r="T6" s="6"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>61</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -2682,8 +2773,8 @@
       <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
@@ -2712,10 +2803,10 @@
       <c r="T8" s="8"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="18" t="s">
@@ -2754,8 +2845,8 @@
       <c r="T9" s="8"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="12" t="s">
         <v>26</v>
       </c>
@@ -2792,10 +2883,10 @@
       <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -2834,8 +2925,8 @@
       <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="12" t="s">
         <v>26</v>
       </c>
@@ -2872,10 +2963,10 @@
       <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -2914,8 +3005,8 @@
       <c r="T13" s="6"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="12" t="s">
         <v>26</v>
       </c>
@@ -2952,10 +3043,10 @@
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="35" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -2992,8 +3083,8 @@
       <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="12" t="s">
         <v>27</v>
       </c>
@@ -3028,10 +3119,10 @@
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>70</v>
       </c>
       <c r="C17" s="18" t="s">
@@ -3074,8 +3165,8 @@
       <c r="T17" s="8"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="36"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12" t="s">
         <v>16</v>
       </c>
@@ -3117,10 +3208,10 @@
       <c r="T18" s="6"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="37" t="s">
         <v>71</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -3163,8 +3254,8 @@
       <c r="T19" s="6"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="12" t="s">
         <v>16</v>
       </c>
@@ -3212,10 +3303,10 @@
       <c r="A23" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="22" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Update positions on investment-transaction changes (#214)
* Update yahoo finance

* Fix updatePosition

* Fix

* Update queue

* Update logs

* Add tests

* Update schema

* Update gitignore

---------

Co-authored-by: Eric Bach <eric.bach@ama.ab.ca>
</commit_message>
<xml_diff>
--- a/references/Tables.xlsx
+++ b/references/Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AMAABCA\eric-bach\pecuniary\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pecuniary\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986B7E23-00A3-4D14-95C2-9AD5AFC781F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3CD9E5-31C8-4896-91D3-81534DF8A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25350" yWindow="1845" windowWidth="26580" windowHeight="18255" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
+    <workbookView xWindow="10530" yWindow="3285" windowWidth="34335" windowHeight="18615" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="9" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
   <si>
     <t>name</t>
   </si>
@@ -453,6 +442,27 @@
   </si>
   <si>
     <t>transaction-gsi</t>
+  </si>
+  <si>
+    <t>bal#&lt;balId&gt;</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>balanceId</t>
+  </si>
+  <si>
+    <t>&lt;balanceId&gt;</t>
+  </si>
+  <si>
+    <t>nw#&lt;networthId&gt;</t>
+  </si>
+  <si>
+    <t>networth</t>
+  </si>
+  <si>
+    <t>divs</t>
   </si>
 </sst>
 </file>
@@ -486,7 +496,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +512,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,7 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -608,9 +624,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -618,33 +647,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -664,9 +677,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -704,7 +717,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -810,7 +823,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -952,7 +965,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -960,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C67D2A-5435-4CFA-A6DE-EEB96100D814}">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A21" sqref="A21:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,25 +999,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
@@ -1016,20 +1029,20 @@
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
@@ -1037,7 +1050,7 @@
       <c r="T2" s="9"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1078,7 +1091,7 @@
       <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
         <v>62</v>
       </c>
@@ -1115,7 +1128,7 @@
       <c r="U4" s="6"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1154,7 +1167,7 @@
       <c r="U5" s="6"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="11" t="s">
         <v>62</v>
       </c>
@@ -1191,7 +1204,7 @@
       <c r="U6" s="6"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="25" t="s">
         <v>67</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1230,7 +1243,7 @@
       <c r="U7" s="6"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="11" t="s">
         <v>62</v>
       </c>
@@ -1267,7 +1280,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -1316,7 +1329,7 @@
       <c r="V9" s="8"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="11" t="s">
         <v>62</v>
       </c>
@@ -1363,7 +1376,7 @@
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1412,7 +1425,7 @@
       <c r="V11" s="6"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="11" t="s">
         <v>62</v>
       </c>
@@ -1459,7 +1472,7 @@
       <c r="V12" s="6"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1508,7 +1521,7 @@
       <c r="V13" s="6"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
         <v>62</v>
       </c>
@@ -1555,7 +1568,7 @@
       <c r="V14" s="6"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1602,7 +1615,7 @@
       <c r="V15" s="6"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
         <v>62</v>
       </c>
@@ -1647,8 +1660,8 @@
       <c r="V16" s="8"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>61</v>
+      <c r="A17" s="25" t="s">
+        <v>132</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>69</v>
@@ -1660,38 +1673,24 @@
         <v>85</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>16</v>
+        <v>133</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="O17" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="28"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="4"/>
@@ -1700,50 +1699,35 @@
       <c r="V17" s="8"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>9</v>
+        <v>135</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1000</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="11">
-        <v>150</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="14">
-        <f>12543+5.99+50*145.23+5.99</f>
-        <v>19816.48</v>
-      </c>
-      <c r="L18" s="14">
-        <v>13458.52</v>
-      </c>
-      <c r="M18" s="14">
-        <v>18617.25</v>
-      </c>
-      <c r="N18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>43</v>
       </c>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="4"/>
@@ -1752,7 +1736,7 @@
       <c r="V18" s="6"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -1788,24 +1772,26 @@
       <c r="L19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="16" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="O19" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="O19" s="16" t="s">
+      <c r="P19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-      <c r="V19" s="6"/>
+      <c r="V19" s="8"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
         <v>62</v>
       </c>
@@ -1819,44 +1805,48 @@
         <v>107</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="H20" s="11">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="14">
-        <f>50*867.23+5.99</f>
-        <v>43367.49</v>
+        <f>12543+5.99+50*145.23+5.99</f>
+        <v>19816.48</v>
       </c>
       <c r="L20" s="14">
-        <v>60215.67</v>
+        <v>13458.52</v>
       </c>
       <c r="M20" s="14">
-        <v>43367.49</v>
-      </c>
-      <c r="N20" s="11" t="s">
+        <v>18617.25</v>
+      </c>
+      <c r="N20" s="11">
+        <v>324.12</v>
+      </c>
+      <c r="O20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20" s="1"/>
+      <c r="P20" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="Q20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
       <c r="V20" s="6"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>108</v>
+      <c r="A21" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>69</v>
@@ -1865,24 +1855,44 @@
         <v>88</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E21" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="O21" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="P21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -1890,38 +1900,59 @@
       <c r="V21" s="6"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="G22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="11">
+        <v>100</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="14">
+        <f>50*867.23+5.99</f>
+        <v>43367.49</v>
+      </c>
+      <c r="L22" s="14">
+        <v>60215.67</v>
+      </c>
+      <c r="M22" s="14">
+        <v>43367.49</v>
+      </c>
+      <c r="N22" s="11">
+        <v>1434.32</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="S22" s="1"/>
       <c r="V22" s="6"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="25" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1939,15 +1970,15 @@
       <c r="F23" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="23"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="10"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="4"/>
@@ -1956,7 +1987,7 @@
       <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="11" t="s">
         <v>62</v>
       </c>
@@ -1964,7 +1995,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>44</v>
@@ -1972,23 +2003,23 @@
       <c r="F24" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="26"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="11"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="S24" s="1"/>
       <c r="V24" s="6"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>110</v>
+      <c r="A25" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>69</v>
@@ -2005,15 +2036,15 @@
       <c r="F25" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="23"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="10"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="4"/>
@@ -2022,15 +2053,15 @@
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>111</v>
+        <v>23</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>44</v>
@@ -2038,23 +2069,23 @@
       <c r="F26" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="25"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="26"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="S26" s="1"/>
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>112</v>
+      <c r="A27" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>69</v>
@@ -2071,15 +2102,15 @@
       <c r="F27" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="23"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="10"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="4"/>
@@ -2088,15 +2119,15 @@
       <c r="V27" s="6"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>44</v>
@@ -2104,39 +2135,159 @@
       <c r="F28" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="25"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="26"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="11"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="S28" s="1"/>
       <c r="V28" s="6"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="D29"/>
+      <c r="A29" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="V29" s="6"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="V30" s="6"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="10"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="32">
+        <v>1204232.1200000001</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
+  <mergeCells count="16">
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B1:O2"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2168,7 +2319,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
+      <c r="A1" s="22"/>
       <c r="B1" s="21" t="s">
         <v>54</v>
       </c>
@@ -2204,68 +2355,68 @@
       </c>
       <c r="M1" s="21"/>
     </row>
-    <row r="2" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="28" t="s">
+    <row r="5" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+    <row r="6" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
       <c r="B6" s="20" t="s">
         <v>80</v>
       </c>
@@ -2278,16 +2429,9 @@
       <c r="E6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-    </row>
-    <row r="7" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+    </row>
+    <row r="7" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
       <c r="B7" s="20" t="s">
         <v>90</v>
       </c>
@@ -2300,104 +2444,90 @@
       <c r="E7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
       <c r="H7" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-    </row>
-    <row r="8" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+    </row>
+    <row r="8" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
     </row>
     <row r="10" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
     </row>
     <row r="11" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">

</xml_diff>

<commit_message>
Add balance field to account
</commit_message>
<xml_diff>
--- a/references/Tables.xlsx
+++ b/references/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pecuniary\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3CD9E5-31C8-4896-91D3-81534DF8A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E34979-764F-4B22-BBCD-FDDD3FA1660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10530" yWindow="3285" windowWidth="34335" windowHeight="18615" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="136">
   <si>
     <t>name</t>
   </si>
@@ -444,16 +444,7 @@
     <t>transaction-gsi</t>
   </si>
   <si>
-    <t>bal#&lt;balId&gt;</t>
-  </si>
-  <si>
     <t>balance</t>
-  </si>
-  <si>
-    <t>balanceId</t>
-  </si>
-  <si>
-    <t>&lt;balanceId&gt;</t>
   </si>
   <si>
     <t>nw#&lt;networthId&gt;</t>
@@ -559,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -632,6 +623,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -639,24 +636,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -973,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C67D2A-5435-4CFA-A6DE-EEB96100D814}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A22"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,8 +966,7 @@
     <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -1002,22 +980,22 @@
       <c r="A1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
@@ -1029,20 +1007,20 @@
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
@@ -1050,7 +1028,7 @@
       <c r="T2" s="9"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1072,26 +1050,29 @@
         <v>0</v>
       </c>
       <c r="H3" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="12"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="3"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="2"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="5"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="11" t="s">
         <v>62</v>
       </c>
@@ -1110,25 +1091,29 @@
       <c r="G4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>37</v>
+      <c r="H4" s="11">
+        <v>213758.85</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="14"/>
+      <c r="M4" s="11"/>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="1"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="1"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-      <c r="U4" s="6"/>
+      <c r="T4" s="4"/>
+      <c r="V4" s="6"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="27" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1150,24 +1135,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="14"/>
+      <c r="M5" s="11"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="1"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="1"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-      <c r="U5" s="6"/>
+      <c r="T5" s="4"/>
+      <c r="V5" s="6"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="11" t="s">
         <v>62</v>
       </c>
@@ -1186,25 +1175,29 @@
       <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>38</v>
+      <c r="H6" s="11">
+        <v>78532.77</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="14"/>
+      <c r="M6" s="11"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="1"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
-      <c r="U6" s="6"/>
+      <c r="T6" s="4"/>
+      <c r="V6" s="6"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>67</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1226,24 +1219,28 @@
         <v>0</v>
       </c>
       <c r="H7" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="14"/>
+      <c r="M7" s="11"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="1"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
-      <c r="U7" s="6"/>
+      <c r="T7" s="4"/>
+      <c r="V7" s="6"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="11" t="s">
         <v>62</v>
       </c>
@@ -1262,25 +1259,29 @@
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>39</v>
+      <c r="H8" s="11">
+        <v>4583.1000000000004</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
-      <c r="M8" s="14"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="1"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="U8" s="8"/>
+      <c r="T8" s="4"/>
+      <c r="V8" s="8"/>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -1329,7 +1330,7 @@
       <c r="V9" s="8"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="11" t="s">
         <v>62</v>
       </c>
@@ -1376,7 +1377,7 @@
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1425,7 +1426,7 @@
       <c r="V11" s="6"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="11" t="s">
         <v>62</v>
       </c>
@@ -1472,7 +1473,7 @@
       <c r="V12" s="6"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1521,7 +1522,7 @@
       <c r="V13" s="6"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="11" t="s">
         <v>62</v>
       </c>
@@ -1568,7 +1569,7 @@
       <c r="V14" s="6"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1615,7 +1616,7 @@
       <c r="V15" s="6"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="11" t="s">
         <v>62</v>
       </c>
@@ -1660,8 +1661,8 @@
       <c r="V16" s="8"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>132</v>
+      <c r="A17" s="27" t="s">
+        <v>61</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>69</v>
@@ -1673,25 +1674,41 @@
         <v>85</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="O17" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="P17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -1699,36 +1716,53 @@
       <c r="V17" s="8"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="11">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="G18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="11">
+        <v>150</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="14">
+        <f>12543+5.99+50*145.23+5.99</f>
+        <v>19816.48</v>
+      </c>
+      <c r="L18" s="14">
+        <v>13458.52</v>
+      </c>
+      <c r="M18" s="14">
+        <v>18617.25</v>
+      </c>
+      <c r="N18" s="11">
+        <v>324.12</v>
+      </c>
+      <c r="O18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="P18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -1736,7 +1770,7 @@
       <c r="V18" s="6"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="27" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -1772,11 +1806,11 @@
       <c r="L19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O19" s="18" t="s">
         <v>109</v>
@@ -1788,10 +1822,10 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-      <c r="V19" s="8"/>
+      <c r="V19" s="6"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="11" t="s">
         <v>62</v>
       </c>
@@ -1805,48 +1839,46 @@
         <v>107</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="H20" s="11">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" s="14">
-        <f>12543+5.99+50*145.23+5.99</f>
-        <v>19816.48</v>
+        <f>50*867.23+5.99</f>
+        <v>43367.49</v>
       </c>
       <c r="L20" s="14">
-        <v>13458.52</v>
+        <v>60215.67</v>
       </c>
       <c r="M20" s="14">
-        <v>18617.25</v>
+        <v>43367.49</v>
       </c>
       <c r="N20" s="11">
-        <v>324.12</v>
+        <v>1434.32</v>
       </c>
       <c r="O20" s="11" t="s">
         <v>42</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="S20" s="1"/>
       <c r="V20" s="6"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>61</v>
+      <c r="A21" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>69</v>
@@ -1855,44 +1887,24 @@
         <v>88</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="O21" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="P21" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -1900,59 +1912,38 @@
       <c r="V21" s="6"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>107</v>
+        <v>23</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="11">
-        <v>100</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K22" s="14">
-        <f>50*867.23+5.99</f>
-        <v>43367.49</v>
-      </c>
-      <c r="L22" s="14">
-        <v>60215.67</v>
-      </c>
-      <c r="M22" s="14">
-        <v>43367.49</v>
-      </c>
-      <c r="N22" s="11">
-        <v>1434.32</v>
-      </c>
-      <c r="O22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="11" t="s">
         <v>44</v>
       </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="S22" s="1"/>
       <c r="V22" s="6"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="27" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1987,7 +1978,7 @@
       <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="11" t="s">
         <v>62</v>
       </c>
@@ -1995,7 +1986,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>44</v>
@@ -2018,8 +2009,8 @@
       <c r="V24" s="6"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>108</v>
+      <c r="A25" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>69</v>
@@ -2053,15 +2044,15 @@
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>44</v>
@@ -2084,8 +2075,8 @@
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>110</v>
+      <c r="A27" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>69</v>
@@ -2119,15 +2110,15 @@
       <c r="V27" s="6"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>44</v>
@@ -2150,8 +2141,8 @@
       <c r="V28" s="6"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>112</v>
+      <c r="A29" s="26" t="s">
+        <v>133</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>69</v>
@@ -2160,7 +2151,7 @@
         <v>88</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>109</v>
@@ -2177,23 +2168,17 @@
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="V29" s="6"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>113</v>
+        <v>134</v>
+      </c>
+      <c r="D30" s="25">
+        <v>1204232.1200000001</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>44</v>
@@ -2210,85 +2195,24 @@
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
       <c r="O30" s="11"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="V30" s="6"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="10"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" s="32">
-        <v>1204232.1200000001</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A31:A32"/>
+  <mergeCells count="15">
+    <mergeCell ref="B1:O2"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B1:O2"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add balance field to account (#215)
* Add balance field to account

* Add updateAccountBalance

* Fix bookValue and ACB calculations

* Update

* Fix types

* Fix

* Fix

* WIP

* Update

* Updates

* Update Readme

* Add tests
</commit_message>
<xml_diff>
--- a/references/Tables.xlsx
+++ b/references/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pecuniary\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3CD9E5-31C8-4896-91D3-81534DF8A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAA9084-B8FB-40BA-A435-EC9A9A4F8E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10530" yWindow="3285" windowWidth="34335" windowHeight="18615" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
+    <workbookView xWindow="4935" yWindow="1650" windowWidth="26685" windowHeight="18765" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="136">
   <si>
     <t>name</t>
   </si>
@@ -444,16 +444,7 @@
     <t>transaction-gsi</t>
   </si>
   <si>
-    <t>bal#&lt;balId&gt;</t>
-  </si>
-  <si>
     <t>balance</t>
-  </si>
-  <si>
-    <t>balanceId</t>
-  </si>
-  <si>
-    <t>&lt;balanceId&gt;</t>
   </si>
   <si>
     <t>nw#&lt;networthId&gt;</t>
@@ -559,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -632,7 +623,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -640,20 +631,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -973,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C67D2A-5435-4CFA-A6DE-EEB96100D814}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A22"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,10 +966,10 @@
     <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="4"/>
     <col min="18" max="18" width="9.140625" style="1"/>
@@ -998,7 +977,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>33</v>
       </c>
@@ -1025,7 +1004,7 @@
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
     </row>
-    <row r="2" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
@@ -1049,8 +1028,8 @@
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1072,26 +1051,32 @@
         <v>0</v>
       </c>
       <c r="H3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
       <c r="B4" s="11" t="s">
         <v>62</v>
       </c>
@@ -1110,25 +1095,31 @@
       <c r="G4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="11">
+        <v>213758.85</v>
+      </c>
+      <c r="I4" s="11">
+        <v>23454335.23</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="1"/>
-      <c r="R4" s="4"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
       <c r="S4" s="4"/>
-      <c r="U4" s="6"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1150,24 +1141,30 @@
         <v>0</v>
       </c>
       <c r="H5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="K5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="1"/>
-      <c r="R5" s="4"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
       <c r="S5" s="4"/>
-      <c r="U5" s="6"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
       <c r="B6" s="11" t="s">
         <v>62</v>
       </c>
@@ -1186,25 +1183,31 @@
       <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="11">
+        <v>78532.77</v>
+      </c>
+      <c r="I6" s="11">
+        <v>124543.23</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="1"/>
-      <c r="R6" s="4"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
       <c r="S6" s="4"/>
-      <c r="U6" s="6"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1226,24 +1229,28 @@
         <v>0</v>
       </c>
       <c r="H7" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="14"/>
+      <c r="M7" s="11"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="1"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
-      <c r="U7" s="6"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="T7" s="4"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
       <c r="B8" s="11" t="s">
         <v>62</v>
       </c>
@@ -1262,25 +1269,29 @@
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>39</v>
+      <c r="H8" s="11">
+        <v>4583.1000000000004</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
-      <c r="M8" s="14"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="1"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="U8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="T8" s="4"/>
+      <c r="V8" s="8"/>
+    </row>
+    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -1328,8 +1339,8 @@
       <c r="T9" s="4"/>
       <c r="V9" s="8"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
       <c r="B10" s="11" t="s">
         <v>62</v>
       </c>
@@ -1375,8 +1386,8 @@
       <c r="T10" s="4"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1424,8 +1435,8 @@
       <c r="T11" s="4"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
       <c r="B12" s="11" t="s">
         <v>62</v>
       </c>
@@ -1471,8 +1482,8 @@
       <c r="T12" s="4"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1520,8 +1531,8 @@
       <c r="T13" s="4"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
       <c r="B14" s="11" t="s">
         <v>62</v>
       </c>
@@ -1567,8 +1578,8 @@
       <c r="T14" s="4"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1614,8 +1625,8 @@
       <c r="T15" s="4"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
       <c r="B16" s="11" t="s">
         <v>62</v>
       </c>
@@ -1660,8 +1671,8 @@
       <c r="V16" s="8"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>132</v>
+      <c r="A17" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>69</v>
@@ -1673,25 +1684,41 @@
         <v>85</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="O17" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="P17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -1699,36 +1726,53 @@
       <c r="V17" s="8"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="11">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="G18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="11">
+        <v>150</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="14">
+        <f>12543+5.99+50*145.23+5.99</f>
+        <v>19816.48</v>
+      </c>
+      <c r="L18" s="14">
+        <v>13458.52</v>
+      </c>
+      <c r="M18" s="14">
+        <v>18617.25</v>
+      </c>
+      <c r="N18" s="11">
+        <v>324.12</v>
+      </c>
+      <c r="O18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="P18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -1736,7 +1780,7 @@
       <c r="V18" s="6"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -1772,11 +1816,11 @@
       <c r="L19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O19" s="18" t="s">
         <v>109</v>
@@ -1788,10 +1832,10 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
-      <c r="V19" s="8"/>
+      <c r="V19" s="6"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="11" t="s">
         <v>62</v>
       </c>
@@ -1805,48 +1849,46 @@
         <v>107</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="H20" s="11">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" s="14">
-        <f>12543+5.99+50*145.23+5.99</f>
-        <v>19816.48</v>
+        <f>50*867.23+5.99</f>
+        <v>43367.49</v>
       </c>
       <c r="L20" s="14">
-        <v>13458.52</v>
+        <v>60215.67</v>
       </c>
       <c r="M20" s="14">
-        <v>18617.25</v>
+        <v>43367.49</v>
       </c>
       <c r="N20" s="11">
-        <v>324.12</v>
+        <v>1434.32</v>
       </c>
       <c r="O20" s="11" t="s">
         <v>42</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="S20" s="1"/>
       <c r="V20" s="6"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>61</v>
+      <c r="A21" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>69</v>
@@ -1855,44 +1897,24 @@
         <v>88</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="O21" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="P21" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -1900,59 +1922,38 @@
       <c r="V21" s="6"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>107</v>
+        <v>23</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="11">
-        <v>100</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K22" s="14">
-        <f>50*867.23+5.99</f>
-        <v>43367.49</v>
-      </c>
-      <c r="L22" s="14">
-        <v>60215.67</v>
-      </c>
-      <c r="M22" s="14">
-        <v>43367.49</v>
-      </c>
-      <c r="N22" s="11">
-        <v>1434.32</v>
-      </c>
-      <c r="O22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="11" t="s">
         <v>44</v>
       </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="S22" s="1"/>
       <c r="V22" s="6"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1987,7 +1988,7 @@
       <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="11" t="s">
         <v>62</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>44</v>
@@ -2018,8 +2019,8 @@
       <c r="V24" s="6"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>108</v>
+      <c r="A25" s="28" t="s">
+        <v>110</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>69</v>
@@ -2053,15 +2054,15 @@
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>44</v>
@@ -2084,8 +2085,8 @@
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>110</v>
+      <c r="A27" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>69</v>
@@ -2119,15 +2120,15 @@
       <c r="V27" s="6"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>44</v>
@@ -2150,8 +2151,8 @@
       <c r="V28" s="6"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>112</v>
+      <c r="A29" s="29" t="s">
+        <v>133</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>69</v>
@@ -2160,7 +2161,7 @@
         <v>88</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>109</v>
@@ -2177,23 +2178,17 @@
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="V29" s="6"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>113</v>
+        <v>134</v>
+      </c>
+      <c r="D30" s="25">
+        <v>1204232.1200000001</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>44</v>
@@ -2210,84 +2205,23 @@
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
       <c r="O30" s="11"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="V30" s="6"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="10"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" s="32">
-        <v>1204232.1200000001</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A31:A32"/>
+  <mergeCells count="15">
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B1:O2"/>
-    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A28"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>